<commit_message>
step 1 is done
Step 1: Determination of partial concordance indices
</commit_message>
<xml_diff>
--- a/data/output_optimiste.xlsx
+++ b/data/output_optimiste.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
   <si>
     <t>categories</t>
   </si>
@@ -35,9 +35,6 @@
   </si>
   <si>
     <t>dumba</t>
-  </si>
-  <si>
-    <t>E</t>
   </si>
   <si>
     <t>A</t>
@@ -430,7 +427,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -438,7 +435,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -446,7 +443,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2">

</xml_diff>